<commit_message>
adds bandwidth robustness check
</commit_message>
<xml_diff>
--- a/Fall 2021/ECON 636V, Communications/mlb_data.xlsx
+++ b/Fall 2021/ECON 636V, Communications/mlb_data.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robbyjeffries/MSEA2022/Fall 2021/ECON 636V, Communications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67AA023-9B21-4142-AF39-209A92E379EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD53D30-E07E-AE4D-8020-36C6FCF8D23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{337FE42C-D1FA-438B-AEF3-6FD22AF9323D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="6" xr2:uid="{337FE42C-D1FA-438B-AEF3-6FD22AF9323D}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="7" r:id="rId1"/>
     <sheet name="Master" sheetId="8" r:id="rId2"/>
+    <sheet name="Experiment" sheetId="9" r:id="rId3"/>
+    <sheet name="Experiment (2)" sheetId="10" r:id="rId4"/>
+    <sheet name="Experiment (3)" sheetId="12" r:id="rId5"/>
+    <sheet name="Experiment (4)" sheetId="13" r:id="rId6"/>
+    <sheet name="Experiment (5)" sheetId="14" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Master!$B$1:$B$998</definedName>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="1035">
   <si>
     <t>Mike Trout</t>
   </si>
@@ -3140,6 +3145,9 @@
   </si>
   <si>
     <t>cumulative</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -3791,8 +3799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C101F75C-1204-4DEB-80CE-6CF33CEF8228}">
   <dimension ref="A1:G998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119:G143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28802,7 +28810,7 @@
         <v>138691970</v>
       </c>
       <c r="F962">
-        <f t="shared" ref="F962:F1025" ca="1" si="30">D962/E962</f>
+        <f t="shared" ref="F962:F998" ca="1" si="30">D962/E962</f>
         <v>4.1884184066316166E-3</v>
       </c>
       <c r="G962" t="str">
@@ -29754,4 +29762,3846 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB8DF84-4CCD-FC43-8671-9E46F6A5DF0A}">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3571687.68</v>
+      </c>
+      <c r="E2" s="3">
+        <f>SUM($D$2:$D$26)</f>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F2">
+        <v>1.1190578030657211E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.98632262685141892</v>
+      </c>
+      <c r="I2">
+        <f>150000000-E2</f>
+        <v>3883007.9999999106</v>
+      </c>
+      <c r="K2" s="3">
+        <f>D2+$I$3</f>
+        <v>3727007.9999999967</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3244687.68</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E26" si="0">SUM($D$2:$D$26)</f>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F3">
+        <v>7.1246680128517568E-3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I3">
+        <f>I2/25</f>
+        <v>155320.31999999643</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K26" si="1">D3+$I$3</f>
+        <v>3400007.9999999967</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3271687.68</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F4">
+        <v>7.4603853537714739E-3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I4">
+        <f>E2+I3</f>
+        <v>146272312.32000008</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="1"/>
+        <v>3427007.9999999967</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4671687.68</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F5">
+        <v>2.4867951179238245E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>4827007.9999999963</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3256687.68</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F6">
+        <v>7.2738757199271864E-3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>3412007.9999999967</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5671687.6799999997</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F7">
+        <v>3.7301926768857366E-2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>5827007.9999999963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3681687.68</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F8">
+        <v>1.2558315345515313E-2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>3837007.9999999967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3571687.68</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F9">
+        <v>1.1190578030657211E-2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>3727007.9999999967</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3">
+        <v>6771687.6799999997</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F10">
+        <v>5.0979299917438402E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>6927007.9999999963</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4771687.68</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F11">
+        <v>2.6111348738200157E-2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>4927007.9999999963</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3264187.68</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F12">
+        <v>7.3671305368493301E-3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>3419507.9999999967</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>26171687.68</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F13">
+        <v>0.29219842635604937</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="1"/>
+        <v>26327007.999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3421687.68</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F14">
+        <v>9.3254816922143415E-3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>3577007.9999999967</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5803987.6799999997</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F15">
+        <v>3.8946941739363979E-2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
+        <v>5959307.9999999963</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3671687.68</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F16">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>3827007.9999999967</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3371687.68</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F17">
+        <v>8.7037829127333856E-3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="1"/>
+        <v>3527007.9999999967</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2">
+        <v>31</v>
+      </c>
+      <c r="D18" s="3">
+        <v>16671687.68</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F18">
+        <v>0.17407565825466773</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="1"/>
+        <v>16827007.999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2">
+        <v>30</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3671687.68</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F19">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="1"/>
+        <v>3827007.9999999967</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3246687.68</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F20">
+        <v>7.1495359640309951E-3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="1"/>
+        <v>3402007.9999999967</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3255687.68</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F21">
+        <v>7.2614417443375677E-3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="1"/>
+        <v>3411007.9999999967</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2">
+        <v>33</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3521687.68</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F22">
+        <v>1.0568879251176255E-2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="1"/>
+        <v>3677007.9999999967</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2">
+        <v>37</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3671687.68</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F23">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="1"/>
+        <v>3827007.9999999967</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2">
+        <v>28</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3264687.68</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F24">
+        <v>7.3733475246441395E-3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="1"/>
+        <v>3420007.9999999967</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="2">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3">
+        <v>9321687.6799999997</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F25">
+        <v>8.2685937670967158E-2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="1"/>
+        <v>9477007.9999999963</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2">
+        <v>28</v>
+      </c>
+      <c r="D26" s="3">
+        <v>11301687.68</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>146116992.00000009</v>
+      </c>
+      <c r="F26">
+        <v>0.10730520933841303</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="1"/>
+        <v>11457007.999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA452D30-AD5A-8641-AD4E-6E990F139599}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3">
+        <v>900000</v>
+      </c>
+      <c r="E2" s="3">
+        <f>SUM($D$2:$D$26)</f>
+        <v>79324800</v>
+      </c>
+      <c r="F2">
+        <v>1.1190578030657211E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.98632262685141892</v>
+      </c>
+      <c r="I2" s="3">
+        <f>AVERAGE(D2:D26)</f>
+        <v>3172992</v>
+      </c>
+      <c r="K2" s="3">
+        <f>D2+$I$3</f>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3">
+        <v>573000</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E26" si="0">SUM($D$2:$D$26)</f>
+        <v>79324800</v>
+      </c>
+      <c r="F3">
+        <v>7.1246680128517568E-3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K26" si="1">D3+$I$3</f>
+        <v>573000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3">
+        <v>600000</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F4">
+        <v>7.4603853537714739E-3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="1"/>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2000000</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F5">
+        <v>2.4867951179238245E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3">
+        <v>585000</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F6">
+        <v>7.2738757199271864E-3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>585000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F7">
+        <v>3.7301926768857366E-2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1010000</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F8">
+        <v>1.2558315345515313E-2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>1010000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3">
+        <v>900000</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F9">
+        <v>1.1190578030657211E-2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4100000</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F10">
+        <v>5.0979299917438402E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>4100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2100000</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F11">
+        <v>2.6111348738200157E-2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>2100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3">
+        <v>592500</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F12">
+        <v>7.3671305368493301E-3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>592500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>23500000</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F13">
+        <v>0.29219842635604937</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="1"/>
+        <v>23500000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3">
+        <v>750000</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F14">
+        <v>9.3254816922143415E-3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3132300</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F15">
+        <v>3.8946941739363979E-2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
+        <v>3132300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F16">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3">
+        <v>700000</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F17">
+        <v>8.7037829127333856E-3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="1"/>
+        <v>700000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2">
+        <v>31</v>
+      </c>
+      <c r="D18" s="3">
+        <v>14000000</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F18">
+        <v>0.17407565825466773</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="1"/>
+        <v>14000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2">
+        <v>30</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F19">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3">
+        <v>575000</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F20">
+        <v>7.1495359640309951E-3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="1"/>
+        <v>575000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3">
+        <v>584000</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F21">
+        <v>7.2614417443375677E-3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="1"/>
+        <v>584000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2">
+        <v>33</v>
+      </c>
+      <c r="D22" s="3">
+        <v>850000</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F22">
+        <v>1.0568879251176255E-2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="1"/>
+        <v>850000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2">
+        <v>37</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F23">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2">
+        <v>28</v>
+      </c>
+      <c r="D24" s="3">
+        <v>593000</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F24">
+        <v>7.3733475246441395E-3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="1"/>
+        <v>593000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="2">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3">
+        <v>6650000</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F25">
+        <v>8.2685937670967158E-2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="1"/>
+        <v>6650000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2">
+        <v>28</v>
+      </c>
+      <c r="D26" s="3">
+        <v>8630000</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F26">
+        <v>0.10730520933841303</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="1"/>
+        <v>8630000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3172992</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28">
+        <v>3172992</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E5FDA3-AE9C-D044-8A8E-A9728D6A1974}">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3">
+        <v>900000</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" ref="E2:E25" si="0">SUM($D$2:$D$25)</f>
+        <v>78751800</v>
+      </c>
+      <c r="F2">
+        <v>1.1190578030657211E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.98632262685141892</v>
+      </c>
+      <c r="I2" s="3">
+        <f>AVERAGE(D2:D25)</f>
+        <v>3281325</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3">
+        <v>600000</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F3">
+        <v>7.4603853537714739E-3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2000000</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F4">
+        <v>2.4867951179238245E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3">
+        <v>585000</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F5">
+        <v>7.2738757199271864E-3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F6">
+        <v>3.7301926768857366E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1010000</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F7">
+        <v>1.2558315345515313E-2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
+        <v>900000</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F8">
+        <v>1.1190578030657211E-2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4100000</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F9">
+        <v>5.0979299917438402E-2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2100000</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F10">
+        <v>2.6111348738200157E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3">
+        <v>592500</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F11">
+        <v>7.3671305368493301E-3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3">
+        <v>23500000</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F12">
+        <v>0.29219842635604937</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3">
+        <v>750000</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F13">
+        <v>9.3254816922143415E-3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2">
+        <v>21</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3132300</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F14">
+        <v>3.8946941739363979E-2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F15">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3">
+        <v>700000</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F16">
+        <v>8.7037829127333856E-3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2">
+        <v>31</v>
+      </c>
+      <c r="D17" s="3">
+        <v>14000000</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F17">
+        <v>0.17407565825466773</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F18">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2">
+        <v>26</v>
+      </c>
+      <c r="D19" s="3">
+        <v>575000</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F19">
+        <v>7.1495359640309951E-3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2">
+        <v>24</v>
+      </c>
+      <c r="D20" s="3">
+        <v>584000</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F20">
+        <v>7.2614417443375677E-3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2">
+        <v>33</v>
+      </c>
+      <c r="D21" s="3">
+        <v>850000</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F21">
+        <v>1.0568879251176255E-2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F22">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2">
+        <v>28</v>
+      </c>
+      <c r="D23" s="3">
+        <v>593000</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F23">
+        <v>7.3733475246441395E-3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2">
+        <v>29</v>
+      </c>
+      <c r="D24" s="3">
+        <v>6650000</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F24">
+        <v>8.2685937670967158E-2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="2">
+        <v>28</v>
+      </c>
+      <c r="D25" s="3">
+        <v>8630000</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>78751800</v>
+      </c>
+      <c r="F25">
+        <v>0.10730520933841303</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F3DD4F-83EC-234A-A851-24F093D93BD6}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3">
+        <v>900000</v>
+      </c>
+      <c r="E2" s="3">
+        <f>SUM($D$2:$D$26)</f>
+        <v>79324800</v>
+      </c>
+      <c r="F2">
+        <v>1.1190578030657211E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.98632262685141892</v>
+      </c>
+      <c r="I2" s="3">
+        <f>AVERAGE(D2:D26)</f>
+        <v>3172992</v>
+      </c>
+      <c r="K2" s="3">
+        <f>D2+$I$3</f>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3">
+        <v>573000</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E26" si="0">SUM($D$2:$D$26)</f>
+        <v>79324800</v>
+      </c>
+      <c r="F3">
+        <v>7.1246680128517568E-3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K26" si="1">D3+$I$3</f>
+        <v>573000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3">
+        <v>600000</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F4">
+        <v>7.4603853537714739E-3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="1"/>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2000000</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F5">
+        <v>2.4867951179238245E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3">
+        <v>585000</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F6">
+        <v>7.2738757199271864E-3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>585000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F7">
+        <v>3.7301926768857366E-2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1010000</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F8">
+        <v>1.2558315345515313E-2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>1010000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3">
+        <v>900000</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F9">
+        <v>1.1190578030657211E-2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4100000</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F10">
+        <v>5.0979299917438402E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>4100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2100000</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F11">
+        <v>2.6111348738200157E-2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>2100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3">
+        <v>592500</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F12">
+        <v>7.3671305368493301E-3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>592500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>23500000</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F13">
+        <v>0.29219842635604937</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="1"/>
+        <v>23500000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3">
+        <v>750000</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F14">
+        <v>9.3254816922143415E-3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3132300</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F15">
+        <v>3.8946941739363979E-2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
+        <v>3132300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F16">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3">
+        <v>700000</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F17">
+        <v>8.7037829127333856E-3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="1"/>
+        <v>700000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2">
+        <v>31</v>
+      </c>
+      <c r="D18" s="3">
+        <v>14000000</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F18">
+        <v>0.17407565825466773</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="1"/>
+        <v>14000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2">
+        <v>30</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F19">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3">
+        <v>575000</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F20">
+        <v>7.1495359640309951E-3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="1"/>
+        <v>575000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3">
+        <v>584000</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F21">
+        <v>7.2614417443375677E-3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="1"/>
+        <v>584000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2">
+        <v>33</v>
+      </c>
+      <c r="D22" s="3">
+        <v>850000</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F22">
+        <v>1.0568879251176255E-2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="1"/>
+        <v>850000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2">
+        <v>37</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F23">
+        <v>1.2433975589619123E-2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2">
+        <v>28</v>
+      </c>
+      <c r="D24" s="3">
+        <v>593000</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F24">
+        <v>7.3733475246441395E-3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="1"/>
+        <v>593000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="2">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3">
+        <v>6650000</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F25">
+        <v>8.2685937670967158E-2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="1"/>
+        <v>6650000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2">
+        <v>28</v>
+      </c>
+      <c r="D26" s="3">
+        <v>8630000</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>79324800</v>
+      </c>
+      <c r="F26">
+        <v>0.10730520933841303</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="1"/>
+        <v>8630000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28">
+        <v>1000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB8C1E0-2C76-044A-91D9-A204186027D8}">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1694203.0739440881</v>
+      </c>
+      <c r="E2">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B2, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F26" ca="1" si="0">D2/E2</f>
+        <v>2.2694209463397022E-2</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G26" ca="1" si="1">IF(B2=B1,"",SUMIF(B:B,B2,F:F))</f>
+        <v>1.7845422637249448</v>
+      </c>
+      <c r="I2" t="e">
+        <f>D2/$D$27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J2" t="e">
+        <f>D2+(I2*$I$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1078642.6237444028</v>
+      </c>
+      <c r="E3">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B3, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4448646691696104E-2</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I3" t="e">
+        <f t="shared" ref="I3:I26" si="2">D3/$D$27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" t="e">
+        <f t="shared" ref="J3:J26" si="3">D3+(I3*$I$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1129468.7159627255</v>
+      </c>
+      <c r="E4">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B4, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5129472975598015E-2</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I4" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3764895.7198757511</v>
+      </c>
+      <c r="E5">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B5, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.043157658532671E-2</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I5" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1101231.9980636572</v>
+      </c>
+      <c r="E6">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B6, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4751236151208063E-2</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5647343.5798136266</v>
+      </c>
+      <c r="E7">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B7, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.5647364877990064E-2</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I7" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1901272.3385372544</v>
+      </c>
+      <c r="E8">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B8, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5467946175589989E-2</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1694203.0739440881</v>
+      </c>
+      <c r="E9">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B9, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2694209463397022E-2</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7718036.2257452905</v>
+      </c>
+      <c r="E10">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B10, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10338473199991977</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3953140.5058695385</v>
+      </c>
+      <c r="E11">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B11, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.2953155414593049E-2</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I11" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1115350.3570131913</v>
+      </c>
+      <c r="E12">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B12, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4940354563403039E-2</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>44237524.708540082</v>
+      </c>
+      <c r="E13">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B13, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.59257102487758895</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1411835.8949534066</v>
+      </c>
+      <c r="E14">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B14, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8911841219497516E-2</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5896391.4316834081</v>
+      </c>
+      <c r="E15">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B15, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.8983413669109437E-2</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I15" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1882447.8599378755</v>
+      </c>
+      <c r="E16">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B16, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5215788292663355E-2</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1317713.5019565132</v>
+      </c>
+      <c r="E17">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B17, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7651051804864353E-2</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I17" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2">
+        <v>31</v>
+      </c>
+      <c r="D18" s="3">
+        <v>26354270.039130259</v>
+      </c>
+      <c r="E18">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B18, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.35302103609728702</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2">
+        <v>30</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1882447.8599378755</v>
+      </c>
+      <c r="E19">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B19, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5215788292663355E-2</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I19" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1082407.5194642786</v>
+      </c>
+      <c r="E20">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B20, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4499078268281432E-2</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I20" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1099349.5502037194</v>
+      </c>
+      <c r="E21">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B21, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.47260203629154E-2</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I21" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2">
+        <v>33</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1600080.6809471943</v>
+      </c>
+      <c r="E22">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B22, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1433420048763856E-2</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2">
+        <v>37</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1882447.8599378755</v>
+      </c>
+      <c r="E23">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B23, Team!$A:$A, 0))</f>
+        <v>74653540</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5215788292663355E-2</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2">
+        <v>28</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1116291.5809431602</v>
+      </c>
+      <c r="E24">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B24, Team!$A:$A, 0))</f>
+        <v>161903375</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.8948011796737419E-3</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I24" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J24" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="2">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3">
+        <v>12518278.268586874</v>
+      </c>
+      <c r="E25">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B25, Team!$A:$A, 0))</f>
+        <v>161903375</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.731943987323843E-2</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I25" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2">
+        <v>28</v>
+      </c>
+      <c r="D26" s="3">
+        <v>16245525.031263866</v>
+      </c>
+      <c r="E26">
+        <f ca="1">INDEX(Team!$B:$B, MATCH(Master!B26, Team!$A:$A, 0))</f>
+        <v>161903375</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10034086708361617</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I26" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <v>70000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>